<commit_message>
update done with register
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8505" windowWidth="18195" xWindow="480" yWindow="60"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,21 +43,83 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -349,16 +407,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tristan</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>394</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>dwfs</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sdfsf</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sdfdsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>onad</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5345</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>kdsj</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update in face recog
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -45,8 +47,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -412,37 +421,127 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="14.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="14.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="2" width="14.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="14.14785714285714"/>
+  </cols>
   <sheetData>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Dedre</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Jano</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>muninginamo</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+    <row customHeight="1" ht="19.5" r="1">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+    </row>
+    <row customHeight="1" ht="19.5" r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>kldfjvks</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>tRIZTAN</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>SDFSF</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>SDFSFD</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="19.5" r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>tRIZTAN</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>2023-05-22</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>01:54:23</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n"/>
+    </row>
+    <row customHeight="1" ht="19.5" r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>tRIZTAN</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>2023-05-22</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>01:58:25</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>tRIZTAN</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>45068.08500893519</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>tRIZTAN</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2023-05-22</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>02:03:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>tRIZTAN</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2023-05-22</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>02:04:25</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>